<commit_message>
adding some ebay test cases
</commit_message>
<xml_diff>
--- a/com.ebay/src/test/resources/TestData.xlsx
+++ b/com.ebay/src/test/resources/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erdosa\IdeaProjects\Selenium_Framework_Team2\com.ebay\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE44BE9-BB5D-4A14-862C-C002D71DE4E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE306AD-98C0-4238-B45F-CE77E039B3C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7005" xr2:uid="{2E8A104B-F2B9-46B0-BA3D-725330091B04}"/>
   </bookViews>
@@ -47,28 +47,28 @@
     <t>Popular destinations</t>
   </si>
   <si>
-    <t>COVID-19</t>
-  </si>
-  <si>
-    <t>Get Started</t>
-  </si>
-  <si>
-    <t>Listing and Marketing</t>
-  </si>
-  <si>
-    <t>Run Your Store</t>
-  </si>
-  <si>
-    <t>Shipping</t>
-  </si>
-  <si>
-    <t>Service and Payments</t>
-  </si>
-  <si>
-    <t>Start Selling</t>
-  </si>
-  <si>
-    <t>Additional Resources</t>
+    <t>Tickets &amp; Experiences</t>
+  </si>
+  <si>
+    <t>Concert Tickets</t>
+  </si>
+  <si>
+    <t>Sports Tickets</t>
+  </si>
+  <si>
+    <t>Theater Tickets</t>
+  </si>
+  <si>
+    <t>Theme Park &amp; Club Passes</t>
+  </si>
+  <si>
+    <t>Parking Passes</t>
+  </si>
+  <si>
+    <t>Special Experiences</t>
+  </si>
+  <si>
+    <t>Other Tickets &amp; Experiences</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>